<commit_message>
"Second Commit for assignment turn in)
</commit_message>
<xml_diff>
--- a/Excel Assignment 2.xlsx
+++ b/Excel Assignment 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryan\Coding Temple\Excel Assignment 2 Budget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD96AEA-6A82-4D84-931D-3F6F2E8AB73F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B009F8BC-66BC-42D5-992A-05BFD5F59E99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="21228" windowHeight="13176" activeTab="1" xr2:uid="{1D6B5232-FB94-4E4F-9AA9-7DC957DC2E0D}"/>
   </bookViews>
@@ -18,6 +18,10 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Data of expenses'!$A$3:$A$67</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'Data of expenses'!$A$3:$A$115</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Data of expenses'!$B$3:$B$115</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Data of expenses'!$A$3:$A$115</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Data of expenses'!$B$3:$B$115</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
@@ -43,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="65">
   <si>
     <t>Budget Form</t>
   </si>
@@ -132,9 +136,6 @@
     <t>groceries</t>
   </si>
   <si>
-    <t>Debts</t>
-  </si>
-  <si>
     <t>Kowalksi</t>
   </si>
   <si>
@@ -183,12 +184,6 @@
     <t>gift</t>
   </si>
   <si>
-    <t>Grocies Expenses</t>
-  </si>
-  <si>
-    <t>Out to eat expenses</t>
-  </si>
-  <si>
     <t>V Look table</t>
   </si>
   <si>
@@ -213,9 +208,6 @@
     <t>Club-Mi</t>
   </si>
   <si>
-    <t>Rent</t>
-  </si>
-  <si>
     <t>Sum of Amount</t>
   </si>
   <si>
@@ -237,52 +229,19 @@
     <t>Source</t>
   </si>
   <si>
-    <t>Insurance is averaged over 6 months its not included in data set</t>
-  </si>
-  <si>
-    <t>Health insurance is not included in data set since its on the employee payroll expense</t>
-  </si>
-  <si>
-    <t>Kids expenses are a cash based system thus not included in the data set</t>
-  </si>
-  <si>
-    <t>Data Hypthosis problems need to improve system by</t>
-  </si>
-  <si>
-    <t>Entertainment seems a bit low the prices must be contained on another data set</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Target is household expenses and groceries so new expense total </t>
-  </si>
-  <si>
-    <t>New Grociers Expense</t>
-  </si>
-  <si>
-    <t>Sums</t>
-  </si>
-  <si>
-    <t>Taking a educated guess on household is 25% of total expense</t>
-  </si>
-  <si>
-    <t>Budget for Grociers</t>
-  </si>
-  <si>
-    <t>Logic Test</t>
-  </si>
-  <si>
-    <t>Budget for Out to eat</t>
-  </si>
-  <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
+    <t>Total Expense</t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>Sum of Expense</t>
+  </si>
+  <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t>Budget for each</t>
   </si>
 </sst>
 </file>
@@ -292,7 +251,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,16 +266,50 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -324,19 +317,55 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="3"/>
+    <xf numFmtId="44" fontId="1" fillId="2" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="5"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="6"/>
+    <xf numFmtId="44" fontId="1" fillId="4" borderId="0" xfId="6" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" pivotButton="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="7">
+    <cellStyle name="20% - Accent1" xfId="6" builtinId="30"/>
+    <cellStyle name="20% - Accent2" xfId="3" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="4" builtinId="50"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Heading 1" xfId="5" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -1532,6 +1561,73 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.0</cx:f>
+      </cx:strDim>
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.1</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Expense by Amount showing high frequence of low totals</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Expense by Amount showing high frequence of low totals</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{ABB70DF5-B3D9-4D1A-9CA9-84E3FED89B18}">
+          <cx:dataLabels pos="inEnd">
+            <cx:visibility seriesName="0" categoryName="0" value="1"/>
+          </cx:dataLabels>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1612,6 +1708,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2634,20 +2770,497 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="371">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800"/>
+    <cs:bodyPr/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="25000"/>
+            <a:lumOff val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1500" b="1" cap="all" spc="100"/>
+    <cs:bodyPr/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>240030</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>598170</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>544830</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>293370</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2674,16 +3287,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>236220</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>556260</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2706,6 +3319,89 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>148590</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Chart 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7396776C-B2B8-D9CD-0C49-C3715398DE53}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3002280" y="335280"/>
+              <a:ext cx="4659630" cy="2987040"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3866,133 +4562,164 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7840E29C-A2AD-4904-9B7E-DA46EEB9EC26}">
-  <dimension ref="A3:L15"/>
+  <dimension ref="A3:D15"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" t="s">
-        <v>57</v>
-      </c>
-      <c r="L3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="11"/>
+    </row>
+    <row r="4" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="2">
+        <v>643.97</v>
+      </c>
+      <c r="C4">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="3">
-        <v>643.97</v>
-      </c>
-      <c r="L4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>18.04</v>
       </c>
-      <c r="L5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>127.91</v>
       </c>
-      <c r="L6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="3">
+        <v>44</v>
+      </c>
+      <c r="B7" s="2">
         <v>26.43</v>
       </c>
-      <c r="L7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>1842.6319999999996</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" s="3">
+        <v>49</v>
+      </c>
+      <c r="B9" s="2">
         <v>12.47</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="3">
+        <v>48</v>
+      </c>
+      <c r="B10" s="2">
         <v>104</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="3">
+        <v>35</v>
+      </c>
+      <c r="B11" s="2">
         <v>384.46</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="3">
+        <v>39</v>
+      </c>
+      <c r="B12" s="2">
         <v>1195</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="2">
+        <v>183.64</v>
+      </c>
+      <c r="C13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="3">
-        <v>183.64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>55</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>60</v>
+      </c>
       <c r="B15" s="1">
         <f>SUM(B4:B14)</f>
         <v>4593.5519999999997</v>
+      </c>
+      <c r="C15">
+        <f>SUM(C4:C14)</f>
+        <v>5000</v>
       </c>
     </row>
   </sheetData>
@@ -4006,7 +4733,7 @@
   <dimension ref="A1:Q115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4014,6 +4741,7 @@
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13.77734375" customWidth="1"/>
     <col min="17" max="17" width="12.88671875" customWidth="1"/>
   </cols>
@@ -4022,1625 +4750,1580 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
-        <v>71</v>
-      </c>
-      <c r="P1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="P1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q1" s="6"/>
+    </row>
+    <row r="2" spans="1:17" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="C2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="P2" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="H2" t="s">
-        <v>69</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="Q2" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="Q2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    </row>
+    <row r="3" spans="1:17" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="4">
         <v>16.05</v>
       </c>
-      <c r="C3" t="str">
+      <c r="C3" s="3" t="str">
         <f>VLOOKUP(A3,P$2:Q$28,2)</f>
         <v>entertainment</v>
       </c>
-      <c r="E3">
-        <f>SUMIF(C3:C115, "=groceries",B3:B115)</f>
-        <v>1842.6319999999996</v>
-      </c>
-      <c r="H3">
-        <f>SUMIF(A3:A115,"=Target",B3:B115)</f>
-        <v>1491.1299999999994</v>
-      </c>
-      <c r="P3" t="s">
+      <c r="P3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="Q3" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="4">
         <v>40.51</v>
       </c>
-      <c r="C4" t="str">
+      <c r="C4" s="3" t="str">
         <f t="shared" ref="C4:C67" si="0">VLOOKUP(A4,P$2:Q$28,2)</f>
         <v>out to eat</v>
       </c>
-      <c r="H4" t="s">
-        <v>72</v>
-      </c>
-      <c r="P4" t="s">
+      <c r="P4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" t="s">
-        <v>42</v>
+      <c r="Q4" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="4">
         <v>45.61</v>
       </c>
-      <c r="C5" t="str">
+      <c r="C5" s="3" t="str">
         <f t="shared" si="0"/>
         <v>gas</v>
       </c>
-      <c r="E5" t="s">
-        <v>47</v>
-      </c>
-      <c r="H5">
-        <f>H3*0.25</f>
-        <v>372.78249999999986</v>
-      </c>
-      <c r="P5" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>36</v>
+      <c r="P5" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="4">
         <v>13.21</v>
       </c>
-      <c r="C6" t="str">
+      <c r="C6" s="3" t="str">
         <f t="shared" si="0"/>
         <v>groceries</v>
       </c>
-      <c r="E6">
-        <f>SUMIF(C3:C115, "=out to eat",B3:B115)</f>
-        <v>384.46</v>
-      </c>
-      <c r="H6" t="s">
-        <v>70</v>
-      </c>
-      <c r="P6" t="s">
+      <c r="P6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="Q6" t="s">
-        <v>43</v>
+      <c r="Q6" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="4">
         <v>55.3</v>
       </c>
-      <c r="C7" t="str">
+      <c r="C7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>groceries</v>
       </c>
-      <c r="H7">
-        <f>E3-H5</f>
-        <v>1469.8494999999998</v>
-      </c>
-      <c r="P7" t="s">
+      <c r="P7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="Q7" t="s">
-        <v>32</v>
+      <c r="Q7" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="4">
         <v>125.72</v>
       </c>
-      <c r="C8" t="str">
+      <c r="C8" s="3" t="str">
         <f t="shared" si="0"/>
         <v>debts</v>
       </c>
-      <c r="E8" t="s">
-        <v>29</v>
-      </c>
-      <c r="P8" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>36</v>
+      <c r="P8" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="4">
         <v>3.78</v>
       </c>
-      <c r="C9" t="str">
+      <c r="C9" s="3" t="str">
         <f t="shared" si="0"/>
         <v>groceries</v>
       </c>
-      <c r="E9">
-        <f>SUMIF(C3:C115,"=debts",B3:B115)</f>
-        <v>643.97</v>
-      </c>
-      <c r="H9" t="s">
-        <v>73</v>
-      </c>
-      <c r="P9" t="s">
+      <c r="P9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="Q9" t="s">
-        <v>36</v>
+      <c r="Q9" s="6" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="4">
         <v>38.14</v>
       </c>
-      <c r="C10" t="str">
+      <c r="C10" s="3" t="str">
         <f t="shared" si="0"/>
         <v>out to eat</v>
       </c>
-      <c r="H10">
-        <v>1500</v>
-      </c>
-      <c r="P10" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q10" t="s">
+      <c r="P10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q10" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="4">
+        <v>1.36</v>
+      </c>
+      <c r="C11" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>groceries</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q11" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="4">
+        <v>3.94</v>
+      </c>
+      <c r="C12" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>groceries</v>
+      </c>
+      <c r="P12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q12" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="4">
+        <v>15.83</v>
+      </c>
+      <c r="C13" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>groceries</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q13" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="4">
+        <v>20</v>
+      </c>
+      <c r="C14" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>groceries</v>
+      </c>
+      <c r="P14" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q14" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="4">
+        <v>20.95</v>
+      </c>
+      <c r="C15" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>groceries</v>
+      </c>
+      <c r="P15" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q15" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="4">
+        <v>52.3</v>
+      </c>
+      <c r="C16" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>groceries</v>
+      </c>
+      <c r="P16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q16" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="4">
+        <v>60.26</v>
+      </c>
+      <c r="C17" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>groceries</v>
+      </c>
+      <c r="P17" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q17" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="4">
+        <v>81.64</v>
+      </c>
+      <c r="C18" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>groceries</v>
+      </c>
+      <c r="P18" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q18" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="4">
+        <v>3.58</v>
+      </c>
+      <c r="C19" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>groceries</v>
+      </c>
+      <c r="P19" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q19" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="4">
+        <v>12.69</v>
+      </c>
+      <c r="C20" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>groceries</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="P20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q20" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="4">
+        <v>69.77</v>
+      </c>
+      <c r="C21" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>groceries</v>
+      </c>
+      <c r="E21" s="8">
+        <v>5000</v>
+      </c>
+      <c r="F21" s="9">
+        <f>SUM(B3:B115)</f>
+        <v>4593.5520000000006</v>
+      </c>
+      <c r="G21" s="8"/>
+      <c r="H21" s="9">
+        <f>E21-F21</f>
+        <v>406.44799999999941</v>
+      </c>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="P21" s="6" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="Q21" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="1">
-        <v>1.36</v>
-      </c>
-      <c r="C11" t="str">
+      <c r="B22" s="4">
+        <v>20.52</v>
+      </c>
+      <c r="C22" s="3" t="str">
         <f t="shared" si="0"/>
         <v>groceries</v>
       </c>
-      <c r="E11" t="s">
-        <v>56</v>
-      </c>
-      <c r="G11" t="s">
-        <v>74</v>
-      </c>
-      <c r="H11" t="str">
-        <f>IF(H7&gt;H10,"out of budget","In budget")</f>
-        <v>In budget</v>
-      </c>
-      <c r="P11" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q11" t="s">
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="P22" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q22" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="1">
-        <v>3.94</v>
-      </c>
-      <c r="C12" t="str">
+      <c r="B23" s="4">
+        <v>42.88</v>
+      </c>
+      <c r="C23" s="3" t="str">
         <f t="shared" si="0"/>
         <v>groceries</v>
       </c>
-      <c r="E12">
-        <f>SUMIF(C3:C115,"=rent",B3:B115)</f>
-        <v>1195</v>
-      </c>
-      <c r="H12" t="s">
-        <v>75</v>
-      </c>
-      <c r="P12" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="1">
-        <v>15.83</v>
-      </c>
-      <c r="C13" t="str">
-        <f t="shared" si="0"/>
-        <v>groceries</v>
-      </c>
-      <c r="H13">
-        <v>400</v>
-      </c>
-      <c r="P13" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="1">
-        <v>20</v>
-      </c>
-      <c r="C14" t="str">
-        <f t="shared" si="0"/>
-        <v>groceries</v>
-      </c>
-      <c r="G14" t="s">
-        <v>74</v>
-      </c>
-      <c r="H14" t="str">
-        <f>IF(E6&gt;H13,"out of budget","In budget")</f>
-        <v>In budget</v>
-      </c>
-      <c r="P14" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="1">
-        <v>20.95</v>
-      </c>
-      <c r="C15" t="str">
-        <f t="shared" si="0"/>
-        <v>groceries</v>
-      </c>
-      <c r="P15" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="1">
-        <v>52.3</v>
-      </c>
-      <c r="C16" t="str">
-        <f t="shared" si="0"/>
-        <v>groceries</v>
-      </c>
-      <c r="P16" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="1">
-        <v>60.26</v>
-      </c>
-      <c r="C17" t="str">
-        <f t="shared" si="0"/>
-        <v>groceries</v>
-      </c>
-      <c r="P17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="1">
-        <v>81.64</v>
-      </c>
-      <c r="C18" t="str">
-        <f t="shared" si="0"/>
-        <v>groceries</v>
-      </c>
-      <c r="P18" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="1">
-        <v>3.58</v>
-      </c>
-      <c r="C19" t="str">
-        <f t="shared" si="0"/>
-        <v>groceries</v>
-      </c>
-      <c r="P19" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="1">
-        <v>12.69</v>
-      </c>
-      <c r="C20" t="str">
-        <f t="shared" si="0"/>
-        <v>groceries</v>
-      </c>
-      <c r="P20" t="s">
+      <c r="P23" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q23" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="1">
-        <v>69.77</v>
-      </c>
-      <c r="C21" t="str">
-        <f t="shared" si="0"/>
-        <v>groceries</v>
-      </c>
-      <c r="P21" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="1">
-        <v>20.52</v>
-      </c>
-      <c r="C22" t="str">
-        <f t="shared" si="0"/>
-        <v>groceries</v>
-      </c>
-      <c r="P22" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="1">
-        <v>42.88</v>
-      </c>
-      <c r="C23" t="str">
-        <f t="shared" si="0"/>
-        <v>groceries</v>
-      </c>
-      <c r="P23" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="A24" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="4">
         <v>4.1900000000000004</v>
       </c>
-      <c r="C24" t="str">
+      <c r="C24" s="3" t="str">
         <f t="shared" si="0"/>
         <v>gas</v>
       </c>
-      <c r="P24" t="s">
+      <c r="P24" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="Q24" t="s">
-        <v>31</v>
+      <c r="Q24" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="A25" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="4">
         <v>105.07</v>
       </c>
-      <c r="C25" t="str">
+      <c r="C25" s="3" t="str">
         <f t="shared" si="0"/>
         <v>groceries</v>
       </c>
-      <c r="P25" t="s">
+      <c r="P25" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="Q25" t="s">
-        <v>45</v>
+      <c r="Q25" s="6" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="A26" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="4">
         <v>2.19</v>
       </c>
-      <c r="C26" t="str">
+      <c r="C26" s="3" t="str">
         <f t="shared" si="0"/>
         <v>groceries</v>
       </c>
-      <c r="P26" t="s">
+      <c r="P26" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="Q26" t="s">
+      <c r="Q26" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="A27" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="4">
         <v>85.13</v>
       </c>
-      <c r="C27" t="str">
+      <c r="C27" s="3" t="str">
         <f t="shared" si="0"/>
         <v>groceries</v>
       </c>
-      <c r="P27" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>36</v>
+      <c r="P27" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q27" s="6" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="A28" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="4">
         <v>29.89</v>
       </c>
-      <c r="C28" t="str">
+      <c r="C28" s="3" t="str">
         <f t="shared" si="0"/>
         <v>out to eat</v>
       </c>
-      <c r="P28" t="s">
+      <c r="P28" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="Q28" t="s">
+      <c r="Q28" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="A29" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="4">
         <v>44.24</v>
       </c>
-      <c r="C29" t="str">
+      <c r="C29" s="3" t="str">
         <f t="shared" si="0"/>
         <v>out to eat</v>
       </c>
-      <c r="P29" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q29" t="s">
+      <c r="P29" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q29" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="A30" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30" s="4">
         <v>59.2</v>
       </c>
-      <c r="C30" t="str">
+      <c r="C30" s="3" t="str">
         <f t="shared" si="0"/>
         <v>debts</v>
       </c>
-      <c r="P30" t="s">
+      <c r="P30" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="Q30" t="s">
-        <v>31</v>
+      <c r="Q30" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>33</v>
-      </c>
-      <c r="B31" s="1">
+      <c r="A31" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="4">
         <v>1.99</v>
       </c>
-      <c r="C31" t="str">
+      <c r="C31" s="3" t="str">
         <f t="shared" si="0"/>
         <v>entertainment</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="A32" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="4">
         <v>6.06</v>
       </c>
-      <c r="C32" t="str">
+      <c r="C32" s="3" t="str">
         <f t="shared" si="0"/>
         <v>gas</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="A33" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33" s="4">
         <v>7.76</v>
       </c>
-      <c r="C33" t="str">
+      <c r="C33" s="3" t="str">
         <f t="shared" si="0"/>
         <v>out to eat</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="A34" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="4">
         <v>5.5</v>
       </c>
-      <c r="C34" t="str">
+      <c r="C34" s="3" t="str">
         <f t="shared" si="0"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="A35" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B35" s="4">
         <v>7.51</v>
       </c>
-      <c r="C35" t="str">
+      <c r="C35" s="3" t="str">
         <f t="shared" si="0"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="A36" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B36" s="4">
         <v>9.17</v>
       </c>
-      <c r="C36" t="str">
+      <c r="C36" s="3" t="str">
         <f t="shared" si="0"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+      <c r="A37" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="4">
         <v>2.56</v>
       </c>
-      <c r="C37" t="str">
+      <c r="C37" s="3" t="str">
         <f t="shared" si="0"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+      <c r="A38" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="4">
         <v>5</v>
       </c>
-      <c r="C38" t="str">
+      <c r="C38" s="3" t="str">
         <f t="shared" si="0"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+      <c r="A39" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="4">
         <v>8.75</v>
       </c>
-      <c r="C39" t="str">
+      <c r="C39" s="3" t="str">
         <f t="shared" si="0"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="A40" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40" s="4">
         <v>11.38</v>
       </c>
-      <c r="C40" t="str">
+      <c r="C40" s="3" t="str">
         <f t="shared" si="0"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+      <c r="A41" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="4">
         <v>13.06</v>
       </c>
-      <c r="C41" t="str">
+      <c r="C41" s="3" t="str">
         <f t="shared" si="0"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+      <c r="A42" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B42" s="1">
+      <c r="B42" s="4">
         <v>32.65</v>
       </c>
-      <c r="C42" t="str">
+      <c r="C42" s="3" t="str">
         <f t="shared" si="0"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+      <c r="A43" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B43" s="4">
         <v>113.37</v>
       </c>
-      <c r="C43" t="str">
+      <c r="C43" s="3" t="str">
         <f t="shared" si="0"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+      <c r="A44" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B44" s="1">
+      <c r="B44" s="4">
         <v>1195</v>
       </c>
-      <c r="C44" t="str">
+      <c r="C44" s="3" t="str">
         <f t="shared" si="0"/>
         <v>rent</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+      <c r="A45" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B45" s="1">
+      <c r="B45" s="4">
         <v>61.92</v>
       </c>
-      <c r="C45" t="str">
+      <c r="C45" s="3" t="str">
         <f t="shared" si="0"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+      <c r="A46" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B46" s="1">
+      <c r="B46" s="4">
         <v>20</v>
       </c>
-      <c r="C46" t="str">
+      <c r="C46" s="3" t="str">
         <f t="shared" si="0"/>
         <v>gas</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+      <c r="A47" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B47" s="1">
+      <c r="B47" s="4">
         <v>45.09</v>
       </c>
-      <c r="C47" t="str">
+      <c r="C47" s="3" t="str">
         <f t="shared" si="0"/>
         <v>out to eat</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+      <c r="A48" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48" s="4">
         <v>6.4</v>
       </c>
-      <c r="C48" t="str">
+      <c r="C48" s="3" t="str">
         <f t="shared" si="0"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+      <c r="A49" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49" s="4">
         <v>8.26</v>
       </c>
-      <c r="C49" t="str">
+      <c r="C49" s="3" t="str">
         <f t="shared" si="0"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="A50" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B50" s="1">
+      <c r="B50" s="4">
         <v>14.13</v>
       </c>
-      <c r="C50" t="str">
+      <c r="C50" s="3" t="str">
         <f t="shared" si="0"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+      <c r="A51" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B51" s="1">
+      <c r="B51" s="4">
         <v>59.41</v>
       </c>
-      <c r="C51" t="str">
+      <c r="C51" s="3" t="str">
         <f t="shared" si="0"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+      <c r="A52" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B52" s="1">
+      <c r="B52" s="4">
         <v>183.64</v>
       </c>
-      <c r="C52" t="str">
+      <c r="C52" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Tools</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+      <c r="A53" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B53" s="1">
+      <c r="B53" s="4">
         <v>7.45</v>
       </c>
-      <c r="C53" t="str">
+      <c r="C53" s="3" t="str">
         <f t="shared" si="0"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+      <c r="A54" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B54" s="1">
+      <c r="B54" s="4">
         <v>12.64</v>
       </c>
-      <c r="C54" t="str">
+      <c r="C54" s="3" t="str">
         <f t="shared" si="0"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+      <c r="A55" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B55" s="1">
+      <c r="B55" s="4">
         <v>13.15</v>
       </c>
-      <c r="C55" t="str">
+      <c r="C55" s="3" t="str">
         <f t="shared" si="0"/>
         <v>out to eat</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+      <c r="A56" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B56" s="1">
+      <c r="B56" s="4">
         <v>32.35</v>
       </c>
-      <c r="C56" t="str">
+      <c r="C56" s="3" t="str">
         <f t="shared" si="0"/>
         <v>out to eat</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
+      <c r="A57" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B57" s="4">
         <v>55</v>
       </c>
-      <c r="C57" t="str">
+      <c r="C57" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ulitities</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+      <c r="A58" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B58" s="4">
         <v>125.72</v>
       </c>
-      <c r="C58" t="str">
+      <c r="C58" s="3" t="str">
         <f t="shared" si="0"/>
         <v>debts</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+      <c r="A59" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B59" s="1">
+      <c r="B59" s="4">
         <v>1.83</v>
       </c>
-      <c r="C59" t="str">
+      <c r="C59" s="3" t="str">
         <f t="shared" si="0"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+      <c r="A60" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B60" s="4">
         <v>2.15</v>
       </c>
-      <c r="C60" t="str">
+      <c r="C60" s="3" t="str">
         <f t="shared" si="0"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+      <c r="A61" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B61" s="1">
+      <c r="B61" s="4">
         <v>12.84</v>
       </c>
-      <c r="C61" t="str">
+      <c r="C61" s="3" t="str">
         <f t="shared" si="0"/>
         <v>out to eat</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
+      <c r="A62" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B62" s="1">
+      <c r="B62" s="4">
         <v>5.01</v>
       </c>
-      <c r="C62" t="str">
+      <c r="C62" s="3" t="str">
         <f t="shared" si="0"/>
         <v>gift</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
+      <c r="A63" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B63" s="1">
+      <c r="B63" s="4">
         <v>4.25</v>
       </c>
-      <c r="C63" t="str">
+      <c r="C63" s="3" t="str">
         <f t="shared" si="0"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+      <c r="A64" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B64" s="1">
+      <c r="B64" s="4">
         <v>15.75</v>
       </c>
-      <c r="C64" t="str">
+      <c r="C64" s="3" t="str">
         <f t="shared" si="0"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
+      <c r="A65" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B65" s="1">
+      <c r="B65" s="4">
         <v>17.920000000000002</v>
       </c>
-      <c r="C65" t="str">
+      <c r="C65" s="3" t="str">
         <f t="shared" si="0"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
+      <c r="A66" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B66" s="1">
+      <c r="B66" s="4">
         <v>20.87</v>
       </c>
-      <c r="C66" t="str">
+      <c r="C66" s="3" t="str">
         <f t="shared" si="0"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
+      <c r="A67" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B67" s="1">
+      <c r="B67" s="4">
         <v>44.86</v>
       </c>
-      <c r="C67" t="str">
+      <c r="C67" s="3" t="str">
         <f t="shared" si="0"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
+      <c r="A68" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B68" s="1">
+      <c r="B68" s="4">
         <v>64.12</v>
       </c>
-      <c r="C68" t="str">
+      <c r="C68" s="3" t="str">
         <f t="shared" ref="C68:C115" si="1">VLOOKUP(A68,P$2:Q$28,2)</f>
         <v>groceries</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
+      <c r="A69" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B69" s="1">
+      <c r="B69" s="4">
         <v>3.84</v>
       </c>
-      <c r="C69" t="str">
+      <c r="C69" s="3" t="str">
         <f t="shared" si="1"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
+      <c r="A70" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B70" s="1">
+      <c r="B70" s="4">
         <v>10</v>
       </c>
-      <c r="C70" t="str">
+      <c r="C70" s="3" t="str">
         <f t="shared" si="1"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>49</v>
-      </c>
-      <c r="B71" s="1">
+      <c r="A71" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B71" s="4">
         <v>12.47</v>
       </c>
-      <c r="C71" t="str">
+      <c r="C71" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Insurance</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>50</v>
-      </c>
-      <c r="B72" s="1">
+      <c r="A72" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B72" s="4">
         <v>52</v>
       </c>
-      <c r="C72" t="str">
+      <c r="C72" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Kids</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>50</v>
-      </c>
-      <c r="B73" s="1">
+      <c r="A73" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B73" s="4">
         <v>52</v>
       </c>
-      <c r="C73" t="str">
+      <c r="C73" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Kids</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
+      <c r="A74" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B74" s="1">
+      <c r="B74" s="4">
         <v>1.31</v>
       </c>
-      <c r="C74" t="str">
+      <c r="C74" s="3" t="str">
         <f t="shared" si="1"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
+      <c r="A75" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B75" s="1">
+      <c r="B75" s="4">
         <v>3.84</v>
       </c>
-      <c r="C75" t="str">
+      <c r="C75" s="3" t="str">
         <f t="shared" si="1"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
+      <c r="A76" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B76" s="1">
+      <c r="B76" s="4">
         <v>54.31</v>
       </c>
-      <c r="C76" t="str">
+      <c r="C76" s="3" t="str">
         <f t="shared" si="1"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
+      <c r="A77" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B77" s="1">
+      <c r="B77" s="4">
         <v>15.69</v>
       </c>
-      <c r="C77" t="str">
+      <c r="C77" s="3" t="str">
         <f t="shared" si="1"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
+      <c r="A78" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B78" s="1">
+      <c r="B78" s="4">
         <v>22.12</v>
       </c>
-      <c r="C78" t="str">
+      <c r="C78" s="3" t="str">
         <f t="shared" si="1"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
+      <c r="A79" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B79" s="1">
+      <c r="B79" s="4">
         <v>29.22</v>
       </c>
-      <c r="C79" t="str">
+      <c r="C79" s="3" t="str">
         <f t="shared" si="1"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
+      <c r="A80" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B80" s="1">
+      <c r="B80" s="4">
         <v>40.86</v>
       </c>
-      <c r="C80" t="str">
+      <c r="C80" s="3" t="str">
         <f t="shared" si="1"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
+      <c r="A81" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B81" s="1">
+      <c r="B81" s="4">
         <v>1.87</v>
       </c>
-      <c r="C81" t="str">
+      <c r="C81" s="3" t="str">
         <f t="shared" si="1"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
+      <c r="A82" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B82" s="1">
+      <c r="B82" s="4">
         <v>5.12</v>
       </c>
-      <c r="C82" t="str">
+      <c r="C82" s="3" t="str">
         <f t="shared" si="1"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
+      <c r="A83" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B83" s="1">
+      <c r="B83" s="4">
         <v>15.14</v>
       </c>
-      <c r="C83" t="str">
+      <c r="C83" s="3" t="str">
         <f t="shared" si="1"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
+      <c r="A84" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B84" s="1">
+      <c r="B84" s="4">
         <v>36.69</v>
       </c>
-      <c r="C84" t="str">
+      <c r="C84" s="3" t="str">
         <f t="shared" si="1"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
+      <c r="A85" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B85" s="1">
+      <c r="B85" s="4">
         <v>12.39</v>
       </c>
-      <c r="C85" t="str">
+      <c r="C85" s="3" t="str">
         <f t="shared" si="1"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>53</v>
-      </c>
-      <c r="B86" s="1">
+      <c r="A86" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B86" s="4">
         <v>26.87</v>
       </c>
-      <c r="C86" t="str">
+      <c r="C86" s="3" t="str">
         <f t="shared" si="1"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>54</v>
-      </c>
-      <c r="B87" s="1">
+      <c r="A87" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B87" s="4">
         <v>11.77</v>
       </c>
-      <c r="C87" t="str">
+      <c r="C87" s="3" t="str">
         <f t="shared" si="1"/>
         <v>out to eat</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>55</v>
-      </c>
-      <c r="B88" s="1">
+      <c r="A88" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B88" s="4">
         <v>22.16</v>
       </c>
-      <c r="C88" t="str">
+      <c r="C88" s="3" t="str">
         <f t="shared" si="1"/>
         <v>out to eat</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
+      <c r="A89" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B89" s="1">
+      <c r="B89" s="4">
         <v>37.799999999999997</v>
       </c>
-      <c r="C89" t="str">
+      <c r="C89" s="3" t="str">
         <f t="shared" si="1"/>
         <v>out to eat</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
-        <v>58</v>
-      </c>
-      <c r="B90" s="1">
+      <c r="A90" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B90" s="4">
         <v>71</v>
       </c>
-      <c r="C90" t="str">
+      <c r="C90" s="3" t="str">
         <f t="shared" si="1"/>
         <v>debts</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
-        <v>58</v>
-      </c>
-      <c r="B91" s="1">
+      <c r="A91" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B91" s="4">
         <v>136.61000000000001</v>
       </c>
-      <c r="C91" t="str">
+      <c r="C91" s="3" t="str">
         <f t="shared" si="1"/>
         <v>debts</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
+      <c r="A92" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B92" s="1">
+      <c r="B92" s="4">
         <v>4.67</v>
       </c>
-      <c r="C92" t="str">
+      <c r="C92" s="3" t="str">
         <f t="shared" si="1"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
-        <v>59</v>
-      </c>
-      <c r="B93" s="1">
+      <c r="A93" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B93" s="4">
         <v>5.55</v>
       </c>
-      <c r="C93" t="str">
+      <c r="C93" s="3" t="str">
         <f t="shared" si="1"/>
         <v>out to eat</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
+      <c r="A94" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B94" s="1">
+      <c r="B94" s="4">
         <v>10.06</v>
       </c>
-      <c r="C94" t="str">
+      <c r="C94" s="3" t="str">
         <f t="shared" si="1"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
+      <c r="A95" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B95" s="1">
+      <c r="B95" s="4">
         <v>10.09</v>
       </c>
-      <c r="C95" t="str">
+      <c r="C95" s="3" t="str">
         <f t="shared" si="1"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
+      <c r="A96" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B96" s="1">
+      <c r="B96" s="4">
         <v>11.47</v>
       </c>
-      <c r="C96" t="str">
+      <c r="C96" s="3" t="str">
         <f t="shared" si="1"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
+      <c r="A97" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B97" s="1">
+      <c r="B97" s="4">
         <v>11.95</v>
       </c>
-      <c r="C97" t="str">
+      <c r="C97" s="3" t="str">
         <f t="shared" si="1"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
+      <c r="A98" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B98" s="1">
+      <c r="B98" s="4">
         <v>21.99</v>
       </c>
-      <c r="C98" t="str">
+      <c r="C98" s="3" t="str">
         <f t="shared" si="1"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
+      <c r="A99" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B99" s="1">
+      <c r="B99" s="4">
         <v>22.88</v>
       </c>
-      <c r="C99" t="str">
+      <c r="C99" s="3" t="str">
         <f t="shared" si="1"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
+      <c r="A100" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B100" s="1">
+      <c r="B100" s="4">
         <v>28.47</v>
       </c>
-      <c r="C100" t="str">
+      <c r="C100" s="3" t="str">
         <f t="shared" si="1"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
+      <c r="A101" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B101" s="1">
+      <c r="B101" s="4">
         <v>70.58</v>
       </c>
-      <c r="C101" t="str">
+      <c r="C101" s="3" t="str">
         <f t="shared" si="1"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
+      <c r="A102" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B102" s="1">
+      <c r="B102" s="4">
         <v>6.69</v>
       </c>
-      <c r="C102" t="str">
+      <c r="C102" s="3" t="str">
         <f t="shared" si="1"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
-        <v>60</v>
-      </c>
-      <c r="B103" s="1">
+      <c r="A103" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B103" s="4">
         <v>7.56</v>
       </c>
-      <c r="C103" t="str">
+      <c r="C103" s="3" t="str">
         <f t="shared" si="1"/>
         <v>out to eat</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
+      <c r="A104" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B104" s="1">
+      <c r="B104" s="4">
         <v>11.85</v>
       </c>
-      <c r="C104" t="str">
+      <c r="C104" s="3" t="str">
         <f t="shared" si="1"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
+      <c r="A105" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B105" s="1">
+      <c r="B105" s="4">
         <v>21.14</v>
       </c>
-      <c r="C105" t="str">
+      <c r="C105" s="3" t="str">
         <f t="shared" si="1"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
+      <c r="A106" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B106" s="1">
+      <c r="B106" s="4">
         <v>21.952000000000002</v>
       </c>
-      <c r="C106" t="str">
+      <c r="C106" s="3" t="str">
         <f t="shared" si="1"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
-        <v>61</v>
-      </c>
-      <c r="B107" s="1">
+      <c r="A107" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B107" s="4">
         <v>18.45</v>
       </c>
-      <c r="C107" t="str">
+      <c r="C107" s="3" t="str">
         <f t="shared" si="1"/>
         <v>out to eat</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
+      <c r="A108" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B108" s="1">
+      <c r="B108" s="4">
         <v>52.05</v>
       </c>
-      <c r="C108" t="str">
+      <c r="C108" s="3" t="str">
         <f t="shared" si="1"/>
         <v>gas</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
-        <v>62</v>
-      </c>
-      <c r="B109" s="1">
+      <c r="A109" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B109" s="4">
         <v>17.2</v>
       </c>
-      <c r="C109" t="str">
+      <c r="C109" s="3" t="str">
         <f t="shared" si="1"/>
         <v>out to eat</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
-        <v>63</v>
-      </c>
-      <c r="B110" s="1">
+      <c r="A110" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B110" s="4">
         <v>21.42</v>
       </c>
-      <c r="C110" t="str">
+      <c r="C110" s="3" t="str">
         <f t="shared" si="1"/>
         <v>gift</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A111" t="s">
+      <c r="A111" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B111" s="1">
+      <c r="B111" s="4">
         <v>10.08</v>
       </c>
-      <c r="C111" t="str">
+      <c r="C111" s="3" t="str">
         <f t="shared" si="1"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
+      <c r="A112" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B112" s="1">
+      <c r="B112" s="4">
         <v>56.63</v>
       </c>
-      <c r="C112" t="str">
+      <c r="C112" s="3" t="str">
         <f t="shared" si="1"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A113" t="s">
+      <c r="A113" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B113" s="1">
+      <c r="B113" s="4">
         <v>125.72</v>
       </c>
-      <c r="C113" t="str">
+      <c r="C113" s="3" t="str">
         <f t="shared" si="1"/>
         <v>debts</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
+      <c r="A114" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B114" s="1">
+      <c r="B114" s="4">
         <v>12.8</v>
       </c>
-      <c r="C114" t="str">
+      <c r="C114" s="3" t="str">
         <f t="shared" si="1"/>
         <v>groceries</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
+      <c r="A115" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B115" s="1">
+      <c r="B115" s="4">
         <v>8.75</v>
       </c>
-      <c r="C115" t="str">
+      <c r="C115" s="3" t="str">
         <f t="shared" si="1"/>
         <v>groceries</v>
       </c>
@@ -5652,5 +6335,6 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>